<commit_message>
Fix chapters module status in tracker - mostly complete
Corrected chapters implementation status:

COMPLETED (functions exist and work):
- extractor.rs: extract_chapters, extract_chapters_to_string, has_chapters
- parser.rs: parse_chapter_xml, serialize_chapter_xml (roxmltree)
- shifter.rs: shift_chapters with clamp/strict modes
- snapper.rs: snap_chapters, extract_keyframes, SnapMode enum
- types.rs: ChapterData, ChapterEntry, KeyframeInfo
- ChaptersStep: Hooked into orchestrator (extract/parse/shift)

NOT HOOKED UP YET:
- snap_chapters() exists but ChaptersStep doesn't call it
- extract_keyframes() exists but ChaptersStep doesn't call it

STILL MISSING:
- _normalize_and_dedupe_chapters (remove duplicates)
- rename_chapters option (Chapter NN format)
- Full ChapLanguageIETF support
</commit_message>
<xml_diff>
--- a/VSG_Rewrite_Tracker.xlsx
+++ b/VSG_Rewrite_Tracker.xlsx
@@ -1127,9 +1127,7 @@
         </is>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" t="inlineStr"/>
-    </row>
+    <row r="37"/>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
@@ -18708,7 +18706,7 @@
       </c>
       <c r="G5" s="16" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Completed</t>
         </is>
       </c>
       <c r="H5" s="16" t="inlineStr">
@@ -18717,8 +18715,16 @@
         </is>
       </c>
       <c r="I5" s="16" t="inlineStr"/>
-      <c r="J5" s="16" t="inlineStr"/>
-      <c r="K5" s="16" t="inlineStr"/>
+      <c r="J5" s="16" t="inlineStr">
+        <is>
+          <t>Keyframe extraction via ffprobe</t>
+        </is>
+      </c>
+      <c r="K5" s="16" t="inlineStr">
+        <is>
+          <t>crates/vsg_core/src/chapters/snapper.rs:78-135</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="16" t="inlineStr"/>
@@ -18745,7 +18751,7 @@
       <c r="F6" s="16" t="inlineStr"/>
       <c r="G6" s="16" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Partial</t>
         </is>
       </c>
       <c r="H6" s="16" t="inlineStr">
@@ -18754,8 +18760,16 @@
         </is>
       </c>
       <c r="I6" s="16" t="inlineStr"/>
-      <c r="J6" s="16" t="inlineStr"/>
-      <c r="K6" s="16" t="inlineStr"/>
+      <c r="J6" s="16" t="inlineStr">
+        <is>
+          <t>XML serialization done. IETF language field partial.</t>
+        </is>
+      </c>
+      <c r="K6" s="16" t="inlineStr">
+        <is>
+          <t>crates/vsg_core/src/chapters/parser.rs:169-235</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="16" t="inlineStr"/>
@@ -18786,7 +18800,7 @@
       </c>
       <c r="G7" s="16" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Partial</t>
         </is>
       </c>
       <c r="H7" s="16" t="inlineStr">
@@ -18795,8 +18809,16 @@
         </is>
       </c>
       <c r="I7" s="16" t="inlineStr"/>
-      <c r="J7" s="16" t="inlineStr"/>
-      <c r="K7" s="16" t="inlineStr"/>
+      <c r="J7" s="16" t="inlineStr">
+        <is>
+          <t>ChapterLanguage parsed. ChapLanguageIETF partial.</t>
+        </is>
+      </c>
+      <c r="K7" s="16" t="inlineStr">
+        <is>
+          <t>crates/vsg_core/src/chapters/parser.rs:148-167</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="16" t="inlineStr"/>
@@ -18827,7 +18849,7 @@
       </c>
       <c r="G8" s="16" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Completed</t>
         </is>
       </c>
       <c r="H8" s="16" t="inlineStr">
@@ -18836,8 +18858,16 @@
         </is>
       </c>
       <c r="I8" s="16" t="inlineStr"/>
-      <c r="J8" s="16" t="inlineStr"/>
-      <c r="K8" s="16" t="inlineStr"/>
+      <c r="J8" s="16" t="inlineStr">
+        <is>
+          <t>Namespace handling via roxmltree</t>
+        </is>
+      </c>
+      <c r="K8" s="16" t="inlineStr">
+        <is>
+          <t>crates/vsg_core/src/chapters/parser.rs</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="16" t="inlineStr"/>
@@ -18864,7 +18894,7 @@
       <c r="F9" s="16" t="inlineStr"/>
       <c r="G9" s="16" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Completed</t>
         </is>
       </c>
       <c r="H9" s="16" t="inlineStr">
@@ -18873,8 +18903,16 @@
         </is>
       </c>
       <c r="I9" s="16" t="inlineStr"/>
-      <c r="J9" s="16" t="inlineStr"/>
-      <c r="K9" s="16" t="inlineStr"/>
+      <c r="J9" s="16" t="inlineStr">
+        <is>
+          <t>Time formatting in types.rs</t>
+        </is>
+      </c>
+      <c r="K9" s="16" t="inlineStr">
+        <is>
+          <t>crates/vsg_core/src/chapters/types.rs:264-274</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="16" t="inlineStr"/>
@@ -18905,7 +18943,7 @@
       </c>
       <c r="G10" s="16" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Completed</t>
         </is>
       </c>
       <c r="H10" s="16" t="inlineStr">
@@ -18914,8 +18952,16 @@
         </is>
       </c>
       <c r="I10" s="16" t="inlineStr"/>
-      <c r="J10" s="16" t="inlineStr"/>
-      <c r="K10" s="16" t="inlineStr"/>
+      <c r="J10" s="16" t="inlineStr">
+        <is>
+          <t>Delta formatting via shifter</t>
+        </is>
+      </c>
+      <c r="K10" s="16" t="inlineStr">
+        <is>
+          <t>crates/vsg_core/src/chapters/shifter.rs</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="16" t="inlineStr"/>
@@ -18946,7 +18992,7 @@
       </c>
       <c r="G11" s="16" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Completed</t>
         </is>
       </c>
       <c r="H11" s="16" t="inlineStr">
@@ -18955,8 +19001,16 @@
         </is>
       </c>
       <c r="I11" s="16" t="inlineStr"/>
-      <c r="J11" s="16" t="inlineStr"/>
-      <c r="K11" s="16" t="inlineStr"/>
+      <c r="J11" s="16" t="inlineStr">
+        <is>
+          <t>Timestamp parsing</t>
+        </is>
+      </c>
+      <c r="K11" s="16" t="inlineStr">
+        <is>
+          <t>crates/vsg_core/src/chapters/types.rs:276-298</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="16" t="inlineStr"/>
@@ -18996,7 +19050,11 @@
         </is>
       </c>
       <c r="I12" s="16" t="inlineStr"/>
-      <c r="J12" s="16" t="inlineStr"/>
+      <c r="J12" s="16" t="inlineStr">
+        <is>
+          <t>Normalization/deduplication not yet implemented</t>
+        </is>
+      </c>
       <c r="K12" s="16" t="inlineStr"/>
     </row>
     <row r="13">
@@ -19024,7 +19082,7 @@
       <c r="F13" s="16" t="inlineStr"/>
       <c r="G13" s="16" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Completed</t>
         </is>
       </c>
       <c r="H13" s="16" t="inlineStr">
@@ -19033,8 +19091,16 @@
         </is>
       </c>
       <c r="I13" s="16" t="inlineStr"/>
-      <c r="J13" s="16" t="inlineStr"/>
-      <c r="K13" s="16" t="inlineStr"/>
+      <c r="J13" s="16" t="inlineStr">
+        <is>
+          <t>Timestamp parsing implemented</t>
+        </is>
+      </c>
+      <c r="K13" s="16" t="inlineStr">
+        <is>
+          <t>crates/vsg_core/src/chapters/types.rs:276-298</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="16" t="inlineStr"/>
@@ -19065,7 +19131,7 @@
       </c>
       <c r="G14" s="16" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Completed</t>
         </is>
       </c>
       <c r="H14" s="16" t="inlineStr">
@@ -19074,8 +19140,16 @@
         </is>
       </c>
       <c r="I14" s="16" t="inlineStr"/>
-      <c r="J14" s="16" t="inlineStr"/>
-      <c r="K14" s="16" t="inlineStr"/>
+      <c r="J14" s="16" t="inlineStr">
+        <is>
+          <t>snap_chapters() with Previous/Nearest/Next modes</t>
+        </is>
+      </c>
+      <c r="K14" s="16" t="inlineStr">
+        <is>
+          <t>crates/vsg_core/src/chapters/snapper.rs:23-65</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="16" t="inlineStr"/>
@@ -19106,7 +19180,7 @@
       </c>
       <c r="G15" s="16" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Completed</t>
         </is>
       </c>
       <c r="H15" s="16" t="inlineStr">
@@ -19115,8 +19189,16 @@
         </is>
       </c>
       <c r="I15" s="16" t="inlineStr"/>
-      <c r="J15" s="16" t="inlineStr"/>
-      <c r="K15" s="16" t="inlineStr"/>
+      <c r="J15" s="16" t="inlineStr">
+        <is>
+          <t>Full chapter processing pipeline in chapters module</t>
+        </is>
+      </c>
+      <c r="K15" s="16" t="inlineStr">
+        <is>
+          <t>crates/vsg_core/src/chapters/</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="16" t="inlineStr"/>
@@ -55541,7 +55623,7 @@
       <c r="I20" s="16" t="inlineStr"/>
       <c r="J20" s="16" t="inlineStr">
         <is>
-          <t>Chapter extraction, shifting, snapping</t>
+          <t>Full ChaptersStep with extraction, parsing, shifting. Snapping implemented but not wired up yet.</t>
         </is>
       </c>
       <c r="K20" s="16" t="inlineStr">
@@ -55590,12 +55672,12 @@
       <c r="I21" s="16" t="inlineStr"/>
       <c r="J21" s="16" t="inlineStr">
         <is>
-          <t>Chapter extraction, shifting, snapping</t>
+          <t>execute() extracts, parses, shifts chapters. Uses chapters module.</t>
         </is>
       </c>
       <c r="K21" s="16" t="inlineStr">
         <is>
-          <t>crates/vsg_core/src/orchestrator/steps/chapters.rs</t>
+          <t>crates/vsg_core/src/orchestrator/steps/chapters.rs:48-137</t>
         </is>
       </c>
     </row>

</xml_diff>